<commit_message>
feat: ustalenie finalnej kolejnosci
</commit_message>
<xml_diff>
--- a/sila-poprawy.xlsx
+++ b/sila-poprawy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedrzejlewandowski/git-repository/lek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E64286-B21D-E040-8814-ED1363CB4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EAE790-9B24-C14C-B61B-7C14B1163A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24940" windowHeight="17640" xr2:uid="{2DE09BD2-B385-E644-A87C-9432D15C5480}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Przedmiot</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Nr 4</t>
+  </si>
+  <si>
+    <t>Nr 5</t>
+  </si>
+  <si>
+    <t>Nr 6</t>
+  </si>
+  <si>
+    <t>Jak starczy czasu przed LEKiem</t>
   </si>
 </sst>
 </file>
@@ -559,7 +568,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <f>D2*(100-C2)/100</f>
+        <f t="shared" ref="E2:E11" si="0">D2*(100-C2)/100</f>
         <v>4</v>
       </c>
       <c r="F2">
@@ -652,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <f>D3*(100-C3)/100</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F3">
@@ -688,7 +697,7 @@
         <v>26</v>
       </c>
       <c r="E4">
-        <f>D4*(100-C4)/100</f>
+        <f t="shared" si="0"/>
         <v>6.9940000000000007</v>
       </c>
       <c r="F4">
@@ -724,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="E5">
-        <f>D5*(100-C5)/100</f>
+        <f t="shared" si="0"/>
         <v>4.2199999999999989</v>
       </c>
       <c r="F5">
@@ -760,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <f>D6*(100-C6)/100</f>
+        <f t="shared" si="0"/>
         <v>3.2339999999999991</v>
       </c>
       <c r="F6">
@@ -796,7 +805,7 @@
         <v>29</v>
       </c>
       <c r="E7">
-        <f>D7*(100-C7)/100</f>
+        <f t="shared" si="0"/>
         <v>6.2060000000000013</v>
       </c>
       <c r="F7">
@@ -832,7 +841,7 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <f>D8*(100-C8)/100</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F8">
@@ -850,7 +859,9 @@
         <f>Table1[[#This Row],[Potencjał]]/(0.45*Table1[[#This Row],[Ilość lekcji]])</f>
         <v>1.6666666666666665</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -866,7 +877,7 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <f>D9*(100-C9)/100</f>
+        <f t="shared" si="0"/>
         <v>3.9959999999999991</v>
       </c>
       <c r="F9">
@@ -884,7 +895,9 @@
         <f>Table1[[#This Row],[Potencjał]]/(0.45*Table1[[#This Row],[Ilość lekcji]])</f>
         <v>1.3199999999999998</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -900,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <f>D10*(100-C10)/100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -918,7 +931,9 @@
         <f>Table1[[#This Row],[Potencjał]]/(0.45*Table1[[#This Row],[Ilość lekcji]])</f>
         <v>0.77777777777777779</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -934,7 +949,7 @@
         <v>39</v>
       </c>
       <c r="E11">
-        <f>D11*(100-C11)/100</f>
+        <f t="shared" si="0"/>
         <v>1.053000000000001</v>
       </c>
       <c r="F11">

</xml_diff>